<commit_message>
Proxy Design pattern examples with approach to simplifies the design pattern to bank and stock market system
</commit_message>
<xml_diff>
--- a/design-patterns-poc/KeyNotes/KeyTakeAways.xlsx
+++ b/design-patterns-poc/KeyNotes/KeyTakeAways.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15480"/>
+    <workbookView windowHeight="15480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1-CreationalDP" sheetId="1" r:id="rId1"/>
@@ -71,6 +71,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Market Data Feed</t>
     </r>
     <r>
@@ -104,6 +112,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Order Type Creation</t>
     </r>
     <r>
@@ -119,6 +135,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Lets subclasses (e.g., </t>
     </r>
     <r>
@@ -158,6 +181,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Multi-Asset Trading</t>
     </r>
     <r>
@@ -191,6 +222,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Portfolio Construction</t>
     </r>
     <r>
@@ -221,6 +260,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Implement </t>
     </r>
     <r>
@@ -266,6 +312,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Clone a Trading Strategy</t>
     </r>
     <r>
@@ -365,6 +419,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Unified Trading Terminal</t>
     </r>
     <r>
@@ -398,6 +460,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Cross-Platform Notifications</t>
     </r>
     <r>
@@ -431,6 +501,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Tax Calculation Pipeline</t>
     </r>
     <r>
@@ -464,6 +542,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Trade Reconciliation System</t>
     </r>
     <r>
@@ -497,6 +583,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Risk Approval Workflow</t>
     </r>
     <r>
@@ -551,6 +645,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Dynamic Fee Calculation</t>
     </r>
     <r>
@@ -605,6 +707,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Order Lifecycle</t>
     </r>
     <r>
@@ -620,6 +730,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Replaces complex </t>
     </r>
     <r>
@@ -659,6 +776,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Portfolio Analytics Engine</t>
     </r>
     <r>
@@ -692,6 +817,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Custom Alert Rules</t>
     </r>
     <r>
@@ -725,6 +858,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF404040"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Portfolio Snapshots</t>
     </r>
     <r>
@@ -930,15 +1071,15 @@
     <font>
       <sz val="10.5"/>
       <color rgb="FF404040"/>
-      <name val="var(--ds-font-family-code)"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10.5"/>
       <color rgb="FF404040"/>
-      <name val="Calibri"/>
+      <name val="var(--ds-font-family-code)"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -956,6 +1097,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1041,12 +1188,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1288,7 +1429,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1312,16 +1453,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1330,42 +1471,42 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1412,7 +1553,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1426,6 +1567,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1961,7 +2105,7 @@
   <sheetPr/>
   <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
@@ -2002,10 +2146,10 @@
       <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2145,8 +2289,8 @@
   <sheetPr/>
   <dimension ref="B2:M13"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -2194,7 +2338,7 @@
       </c>
     </row>
     <row r="4" ht="106" spans="2:8">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -2217,7 +2361,7 @@
       </c>
     </row>
     <row r="5" ht="71" spans="2:10">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -2311,9 +2455,9 @@
         <v>78</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" ht="17.6" spans="10:11">
       <c r="J9" s="4"/>
@@ -2418,7 +2562,7 @@
       <c r="J4" s="4"/>
       <c r="L4" s="4"/>
     </row>
-    <row r="5" ht="159" spans="2:12">
+    <row r="5" ht="88" spans="2:12">
       <c r="B5" s="2" t="s">
         <v>86</v>
       </c>
@@ -2443,7 +2587,7 @@
       <c r="J5" s="4"/>
       <c r="L5" s="4"/>
     </row>
-    <row r="6" ht="159" spans="2:12">
+    <row r="6" ht="88" spans="2:12">
       <c r="B6" s="2" t="s">
         <v>93</v>
       </c>
@@ -2468,7 +2612,7 @@
       <c r="J6" s="4"/>
       <c r="L6" s="4"/>
     </row>
-    <row r="7" ht="124" spans="2:12">
+    <row r="7" ht="106" spans="2:12">
       <c r="B7" s="2" t="s">
         <v>100</v>
       </c>
@@ -2493,7 +2637,7 @@
       <c r="J7" s="4"/>
       <c r="L7" s="4"/>
     </row>
-    <row r="8" ht="141" spans="2:12">
+    <row r="8" ht="88" spans="2:12">
       <c r="B8" s="2" t="s">
         <v>107</v>
       </c>
@@ -2518,7 +2662,7 @@
       <c r="J8" s="4"/>
       <c r="L8" s="4"/>
     </row>
-    <row r="9" ht="124" spans="2:12">
+    <row r="9" ht="88" spans="2:12">
       <c r="B9" s="2" t="s">
         <v>114</v>
       </c>
@@ -2542,7 +2686,7 @@
       </c>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" ht="139" spans="2:12">
+    <row r="10" ht="88" spans="2:12">
       <c r="B10" s="2" t="s">
         <v>121</v>
       </c>
@@ -2566,7 +2710,7 @@
       </c>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" ht="159" spans="2:12">
+    <row r="11" ht="88" spans="2:12">
       <c r="B11" s="2" t="s">
         <v>128</v>
       </c>
@@ -2590,7 +2734,7 @@
       </c>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" ht="176" spans="2:12">
+    <row r="12" ht="88" spans="2:12">
       <c r="B12" s="2" t="s">
         <v>135</v>
       </c>
@@ -2614,7 +2758,7 @@
       </c>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" ht="159" spans="2:12">
+    <row r="13" ht="88" spans="2:12">
       <c r="B13" s="2" t="s">
         <v>142</v>
       </c>

</xml_diff>

<commit_message>
Refactor the code base
</commit_message>
<xml_diff>
--- a/design-patterns-poc/KeyNotes/KeyTakeAways.xlsx
+++ b/design-patterns-poc/KeyNotes/KeyTakeAways.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15480" activeTab="1"/>
+    <workbookView windowHeight="15480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="1-CreationalDP" sheetId="1" r:id="rId1"/>
     <sheet name="2-StructuralDP" sheetId="2" r:id="rId2"/>
     <sheet name="3-BehaviouralDP" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="209">
   <si>
     <t>Creational Patterns</t>
   </si>
@@ -881,6 +882,186 @@
   </si>
   <si>
     <t>Captures state before hypothetical trades.</t>
+  </si>
+  <si>
+    <t>𝐖𝐡𝐲 𝐃𝐞𝐬𝐢𝐠𝐧 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬 𝐌𝐚𝐭𝐭𝐞𝐫?</t>
+  </si>
+  <si>
+    <t>[1.] Reusability</t>
+  </si>
+  <si>
+    <t>◾ proven solutions that work across projects</t>
+  </si>
+  <si>
+    <t>[2.] Flexibility</t>
+  </si>
+  <si>
+    <t>◾ encourage loose coupling and easier maintenance</t>
+  </si>
+  <si>
+    <t>[3.] Communication</t>
+  </si>
+  <si>
+    <t>◾ provide a shared vocabulary for discussing design issues and solutions</t>
+  </si>
+  <si>
+    <t>[4.] Experience</t>
+  </si>
+  <si>
+    <t>◾ encapsulate the experience of seasoned developers, helping others avoid common pitfalls and design better software</t>
+  </si>
+  <si>
+    <t>📌 𝐂𝐫𝐞𝐚𝐭𝐢𝐨𝐧𝐚𝐥 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬</t>
+  </si>
+  <si>
+    <t>[1.] Abstract Factory</t>
+  </si>
+  <si>
+    <t>◾ creates families of related objects through a common interface</t>
+  </si>
+  <si>
+    <t>[2.] Builder</t>
+  </si>
+  <si>
+    <t>◾ separates complex object construction from representation</t>
+  </si>
+  <si>
+    <t>[3.] Factory Method</t>
+  </si>
+  <si>
+    <t>◾ defines an interface for creating objects</t>
+  </si>
+  <si>
+    <t>◾ allows subclasses to choose the concrete class to instantiate</t>
+  </si>
+  <si>
+    <t>[4.] Prototype</t>
+  </si>
+  <si>
+    <t>◾ creates new objects by copying a prototypical instance</t>
+  </si>
+  <si>
+    <t>[5.] Singleton</t>
+  </si>
+  <si>
+    <t>◾ ensures a class has only one instance</t>
+  </si>
+  <si>
+    <t>📌 𝐒𝐭𝐫𝐮𝐜𝐭𝐮𝐫𝐚𝐥 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬</t>
+  </si>
+  <si>
+    <t>[6.] Adapter</t>
+  </si>
+  <si>
+    <t>◾ converts one interface to another, allowing incompatible classes to work together</t>
+  </si>
+  <si>
+    <t>[7.] Bridge</t>
+  </si>
+  <si>
+    <t>◾ decouples abstraction and implementation, enabling independent variation</t>
+  </si>
+  <si>
+    <t>[8.] Composite</t>
+  </si>
+  <si>
+    <t>◾ treats individual objects &amp; their compositions uniformly, representing part-whole hierarchies</t>
+  </si>
+  <si>
+    <t>[9.] Decorator</t>
+  </si>
+  <si>
+    <t>◾ dynamically adds responsibilities to an object without subclassing</t>
+  </si>
+  <si>
+    <t>[10.] Facade</t>
+  </si>
+  <si>
+    <t>◾ provides a simplified interface to a complex subsystem</t>
+  </si>
+  <si>
+    <t>[11.] Flyweight</t>
+  </si>
+  <si>
+    <t>◾ shares objects to reduce memory usage for large numbers of fine-grained objects</t>
+  </si>
+  <si>
+    <t>[12.] Proxy</t>
+  </si>
+  <si>
+    <t>◾ controls access to an object, offering various capabilities like lazy loading or remote access</t>
+  </si>
+  <si>
+    <t>📌 𝐁𝐞𝐡𝐚𝐯𝐢𝐨𝐫𝐚𝐥 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬</t>
+  </si>
+  <si>
+    <t>[13.] Chain of Responsibility</t>
+  </si>
+  <si>
+    <t>◾ decouples request senders and receivers, allowing multiple objects to handle the request</t>
+  </si>
+  <si>
+    <t>[14.] Command</t>
+  </si>
+  <si>
+    <t>◾ encapsulates requests as objects, enabling logging, queuing, and undo/redo operations</t>
+  </si>
+  <si>
+    <t>[15.] Interpreter</t>
+  </si>
+  <si>
+    <t>◾ defines a grammar for a language and an interpreter to execute expressions</t>
+  </si>
+  <si>
+    <t>[16.] Iterator</t>
+  </si>
+  <si>
+    <t>◾ provides sequential access to aggregate elements without exposing the underlying representation</t>
+  </si>
+  <si>
+    <t>[17.] Mediator</t>
+  </si>
+  <si>
+    <t>◾ encapsulates object interaction, promoting loose coupling</t>
+  </si>
+  <si>
+    <t>[18.] Memento</t>
+  </si>
+  <si>
+    <t>◾ captures and restores an object's state without violating encapsulation</t>
+  </si>
+  <si>
+    <t>[19.] Observer</t>
+  </si>
+  <si>
+    <t>◾ notifies dependents automatically when an object's state changes</t>
+  </si>
+  <si>
+    <t>[20.] State</t>
+  </si>
+  <si>
+    <t>◾ alters an object's behavior when its internal state changes</t>
+  </si>
+  <si>
+    <t>[21.] Strategy</t>
+  </si>
+  <si>
+    <t>◾ encapsulates interchangeable algorithms, allowing clients to choose dynamically</t>
+  </si>
+  <si>
+    <t>[22.] Template</t>
+  </si>
+  <si>
+    <t>◾ defines the skeleton of an algorithm, deferring steps to subclasses</t>
+  </si>
+  <si>
+    <t>[23.] Visitor</t>
+  </si>
+  <si>
+    <t>◾ adds new operations to object structures without modifying the element classes</t>
+  </si>
+  <si>
+    <t>While design patterns are conceptual, their proper application is often reflected in consistent structure, naming, and abstraction. Tools like CodeRabbit help catch inconsistencies and code smells during reviews, making it easier to maintain pattern-aligned code as projects scale.</t>
   </si>
 </sst>
 </file>
@@ -893,9 +1074,16 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1071,18 +1259,18 @@
     <font>
       <sz val="10.5"/>
       <color rgb="FF404040"/>
+      <name val="var(--ds-font-family-code)"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF404040"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10.5"/>
-      <color rgb="FF404040"/>
-      <name val="var(--ds-font-family-code)"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1092,6 +1280,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1423,55 +1617,52 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1486,96 +1677,105 @@
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1853,6 +2053,53 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>650240</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="No alternative text description for this image"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1" r:link="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1463040" y="426720"/>
+          <a:ext cx="10160000" cy="11849100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="WPS">
   <a:themeElements>
@@ -2105,8 +2352,8 @@
   <sheetPr/>
   <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -2120,160 +2367,160 @@
   </cols>
   <sheetData>
     <row r="2" ht="19.2" spans="2:8">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" ht="36" spans="2:8">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" ht="106" spans="2:8">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" ht="106" spans="2:10">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" ht="88" spans="2:10">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" ht="106" spans="2:10">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="4"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" ht="88" spans="2:10">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" ht="17.6" spans="10:10">
-      <c r="J9" s="4"/>
+      <c r="J9" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2289,8 +2536,8 @@
   <sheetPr/>
   <dimension ref="B2:M13"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -2304,176 +2551,176 @@
   </cols>
   <sheetData>
     <row r="2" ht="19.2" spans="2:8">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" ht="36" spans="2:8">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" ht="106" spans="2:8">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" ht="71" spans="2:10">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="4"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" ht="71" spans="2:10">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" ht="88" spans="2:10">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J7" s="4"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" ht="88" spans="2:13">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" ht="17.6" spans="10:11">
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" ht="17.6" spans="11:11">
-      <c r="K10" s="4"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" ht="17.6" spans="11:11">
-      <c r="K11" s="4"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" ht="17.6" spans="11:11">
-      <c r="K12" s="4"/>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" ht="17.6" spans="11:11">
-      <c r="K13" s="4"/>
+      <c r="K13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2490,7 +2737,7 @@
   <dimension ref="B2:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -2504,283 +2751,283 @@
   </cols>
   <sheetData>
     <row r="2" ht="19.2" spans="2:8">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" ht="36" spans="2:8">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" ht="88" spans="2:12">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="L4" s="4"/>
+      <c r="J4" s="6"/>
+      <c r="L4" s="6"/>
     </row>
     <row r="5" ht="88" spans="2:12">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="J5" s="6"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6" ht="88" spans="2:12">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="J6" s="6"/>
+      <c r="L6" s="6"/>
     </row>
     <row r="7" ht="106" spans="2:12">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="J7" s="6"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" ht="88" spans="2:12">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="J8" s="6"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" ht="88" spans="2:12">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" ht="88" spans="2:12">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="L10" s="4"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" ht="88" spans="2:12">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="L11" s="4"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" ht="88" spans="2:12">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="L12" s="4"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" ht="88" spans="2:12">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="L13" s="4"/>
+      <c r="L13" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2789,4 +3036,325 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="R3:R86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3:R86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetData>
+    <row r="3" spans="18:18">
+      <c r="R3" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="18:18">
+      <c r="R4" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="18:18">
+      <c r="R5" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="18:18">
+      <c r="R6" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="18:18">
+      <c r="R7" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="18:18">
+      <c r="R8" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="18:18">
+      <c r="R9" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="18:18">
+      <c r="R10" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="18:18">
+      <c r="R11" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="18:18">
+      <c r="R13" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="18:18">
+      <c r="R14" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="18:18">
+      <c r="R15" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="18:18">
+      <c r="R17" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="18:18">
+      <c r="R18" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="18:18">
+      <c r="R20" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="18:18">
+      <c r="R21" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="18:18">
+      <c r="R22" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="18:18">
+      <c r="R24" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="18:18">
+      <c r="R25" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="18:18">
+      <c r="R27" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="18:18">
+      <c r="R28" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="18:18">
+      <c r="R30" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="18:18">
+      <c r="R31" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="18:18">
+      <c r="R32" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="18:18">
+      <c r="R34" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="18:18">
+      <c r="R35" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="18:18">
+      <c r="R37" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="18:18">
+      <c r="R38" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="40" spans="18:18">
+      <c r="R40" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="18:18">
+      <c r="R41" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43" spans="18:18">
+      <c r="R43" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="44" spans="18:18">
+      <c r="R44" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="18:18">
+      <c r="R46" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="18:18">
+      <c r="R47" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="18:18">
+      <c r="R49" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="18:18">
+      <c r="R50" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="52" spans="18:18">
+      <c r="R52" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="53" spans="18:18">
+      <c r="R53" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="54" spans="18:18">
+      <c r="R54" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="18:18">
+      <c r="R56" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="18:18">
+      <c r="R57" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="59" spans="18:18">
+      <c r="R59" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="18:18">
+      <c r="R60" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="18:18">
+      <c r="R62" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="18:18">
+      <c r="R63" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="65" spans="18:18">
+      <c r="R65" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="66" spans="18:18">
+      <c r="R66" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="18:18">
+      <c r="R68" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="18:18">
+      <c r="R69" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="18:18">
+      <c r="R71" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="18:18">
+      <c r="R72" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="74" spans="18:18">
+      <c r="R74" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75" spans="18:18">
+      <c r="R75" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="77" spans="18:18">
+      <c r="R77" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="18:18">
+      <c r="R78" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="80" spans="18:18">
+      <c r="R80" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="81" spans="18:18">
+      <c r="R81" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="83" spans="18:18">
+      <c r="R83" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="84" spans="18:18">
+      <c r="R84" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="86" spans="18:18">
+      <c r="R86" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R86" r:id="rId2" display="While design patterns are conceptual, their proper application is often reflected in consistent structure, naming, and abstraction. Tools like CodeRabbit help catch inconsistencies and code smells during reviews, making it easier to maintain pattern-aligned code as projects scale." tooltip="https://www.linkedin.com/company/coderabbitai/"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the notes. Related to all design patterns.
</commit_message>
<xml_diff>
--- a/design-patterns-poc/KeyNotes/KeyTakeAways.xlsx
+++ b/design-patterns-poc/KeyNotes/KeyTakeAways.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15480" activeTab="3"/>
+    <workbookView windowHeight="15480"/>
   </bookViews>
   <sheets>
-    <sheet name="1-CreationalDP" sheetId="1" r:id="rId1"/>
-    <sheet name="2-StructuralDP" sheetId="2" r:id="rId2"/>
-    <sheet name="3-BehaviouralDP" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Summery" sheetId="4" r:id="rId1"/>
+    <sheet name="1-CreationalDP" sheetId="1" r:id="rId2"/>
+    <sheet name="2-StructuralDP" sheetId="2" r:id="rId3"/>
+    <sheet name="3-BehaviouralDP" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,6 +32,186 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="209">
   <si>
+    <t>𝐖𝐡𝐲 𝐃𝐞𝐬𝐢𝐠𝐧 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬 𝐌𝐚𝐭𝐭𝐞𝐫?</t>
+  </si>
+  <si>
+    <t>[1.] Reusability</t>
+  </si>
+  <si>
+    <t>◾ proven solutions that work across projects</t>
+  </si>
+  <si>
+    <t>[2.] Flexibility</t>
+  </si>
+  <si>
+    <t>◾ encourage loose coupling and easier maintenance</t>
+  </si>
+  <si>
+    <t>[3.] Communication</t>
+  </si>
+  <si>
+    <t>◾ provide a shared vocabulary for discussing design issues and solutions</t>
+  </si>
+  <si>
+    <t>[4.] Experience</t>
+  </si>
+  <si>
+    <t>◾ encapsulate the experience of seasoned developers, helping others avoid common pitfalls and design better software</t>
+  </si>
+  <si>
+    <t>📌 𝐂𝐫𝐞𝐚𝐭𝐢𝐨𝐧𝐚𝐥 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬</t>
+  </si>
+  <si>
+    <t>[1.] Abstract Factory</t>
+  </si>
+  <si>
+    <t>◾ creates families of related objects through a common interface</t>
+  </si>
+  <si>
+    <t>[2.] Builder</t>
+  </si>
+  <si>
+    <t>◾ separates complex object construction from representation</t>
+  </si>
+  <si>
+    <t>[3.] Factory Method</t>
+  </si>
+  <si>
+    <t>◾ defines an interface for creating objects</t>
+  </si>
+  <si>
+    <t>◾ allows subclasses to choose the concrete class to instantiate</t>
+  </si>
+  <si>
+    <t>[4.] Prototype</t>
+  </si>
+  <si>
+    <t>◾ creates new objects by copying a prototypical instance</t>
+  </si>
+  <si>
+    <t>[5.] Singleton</t>
+  </si>
+  <si>
+    <t>◾ ensures a class has only one instance</t>
+  </si>
+  <si>
+    <t>📌 𝐒𝐭𝐫𝐮𝐜𝐭𝐮𝐫𝐚𝐥 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬</t>
+  </si>
+  <si>
+    <t>[6.] Adapter</t>
+  </si>
+  <si>
+    <t>◾ converts one interface to another, allowing incompatible classes to work together</t>
+  </si>
+  <si>
+    <t>[7.] Bridge</t>
+  </si>
+  <si>
+    <t>◾ decouples abstraction and implementation, enabling independent variation</t>
+  </si>
+  <si>
+    <t>[8.] Composite</t>
+  </si>
+  <si>
+    <t>◾ treats individual objects &amp; their compositions uniformly, representing part-whole hierarchies</t>
+  </si>
+  <si>
+    <t>[9.] Decorator</t>
+  </si>
+  <si>
+    <t>◾ dynamically adds responsibilities to an object without subclassing</t>
+  </si>
+  <si>
+    <t>[10.] Facade</t>
+  </si>
+  <si>
+    <t>◾ provides a simplified interface to a complex subsystem</t>
+  </si>
+  <si>
+    <t>[11.] Flyweight</t>
+  </si>
+  <si>
+    <t>◾ shares objects to reduce memory usage for large numbers of fine-grained objects</t>
+  </si>
+  <si>
+    <t>[12.] Proxy</t>
+  </si>
+  <si>
+    <t>◾ controls access to an object, offering various capabilities like lazy loading or remote access</t>
+  </si>
+  <si>
+    <t>📌 𝐁𝐞𝐡𝐚𝐯𝐢𝐨𝐫𝐚𝐥 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬</t>
+  </si>
+  <si>
+    <t>[13.] Chain of Responsibility</t>
+  </si>
+  <si>
+    <t>◾ decouples request senders and receivers, allowing multiple objects to handle the request</t>
+  </si>
+  <si>
+    <t>[14.] Command</t>
+  </si>
+  <si>
+    <t>◾ encapsulates requests as objects, enabling logging, queuing, and undo/redo operations</t>
+  </si>
+  <si>
+    <t>[15.] Interpreter</t>
+  </si>
+  <si>
+    <t>◾ defines a grammar for a language and an interpreter to execute expressions</t>
+  </si>
+  <si>
+    <t>[16.] Iterator</t>
+  </si>
+  <si>
+    <t>◾ provides sequential access to aggregate elements without exposing the underlying representation</t>
+  </si>
+  <si>
+    <t>[17.] Mediator</t>
+  </si>
+  <si>
+    <t>◾ encapsulates object interaction, promoting loose coupling</t>
+  </si>
+  <si>
+    <t>[18.] Memento</t>
+  </si>
+  <si>
+    <t>◾ captures and restores an object's state without violating encapsulation</t>
+  </si>
+  <si>
+    <t>[19.] Observer</t>
+  </si>
+  <si>
+    <t>◾ notifies dependents automatically when an object's state changes</t>
+  </si>
+  <si>
+    <t>[20.] State</t>
+  </si>
+  <si>
+    <t>◾ alters an object's behavior when its internal state changes</t>
+  </si>
+  <si>
+    <t>[21.] Strategy</t>
+  </si>
+  <si>
+    <t>◾ encapsulates interchangeable algorithms, allowing clients to choose dynamically</t>
+  </si>
+  <si>
+    <t>[22.] Template</t>
+  </si>
+  <si>
+    <t>◾ defines the skeleton of an algorithm, deferring steps to subclasses</t>
+  </si>
+  <si>
+    <t>[23.] Visitor</t>
+  </si>
+  <si>
+    <t>◾ adds new operations to object structures without modifying the element classes</t>
+  </si>
+  <si>
+    <t>While design patterns are conceptual, their proper application is often reflected in consistent structure, naming, and abstraction. Tools like CodeRabbit help catch inconsistencies and code smells during reviews, making it easier to maintain pattern-aligned code as projects scale.</t>
+  </si>
+  <si>
     <t>Creational Patterns</t>
   </si>
   <si>
@@ -882,186 +1062,6 @@
   </si>
   <si>
     <t>Captures state before hypothetical trades.</t>
-  </si>
-  <si>
-    <t>𝐖𝐡𝐲 𝐃𝐞𝐬𝐢𝐠𝐧 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬 𝐌𝐚𝐭𝐭𝐞𝐫?</t>
-  </si>
-  <si>
-    <t>[1.] Reusability</t>
-  </si>
-  <si>
-    <t>◾ proven solutions that work across projects</t>
-  </si>
-  <si>
-    <t>[2.] Flexibility</t>
-  </si>
-  <si>
-    <t>◾ encourage loose coupling and easier maintenance</t>
-  </si>
-  <si>
-    <t>[3.] Communication</t>
-  </si>
-  <si>
-    <t>◾ provide a shared vocabulary for discussing design issues and solutions</t>
-  </si>
-  <si>
-    <t>[4.] Experience</t>
-  </si>
-  <si>
-    <t>◾ encapsulate the experience of seasoned developers, helping others avoid common pitfalls and design better software</t>
-  </si>
-  <si>
-    <t>📌 𝐂𝐫𝐞𝐚𝐭𝐢𝐨𝐧𝐚𝐥 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬</t>
-  </si>
-  <si>
-    <t>[1.] Abstract Factory</t>
-  </si>
-  <si>
-    <t>◾ creates families of related objects through a common interface</t>
-  </si>
-  <si>
-    <t>[2.] Builder</t>
-  </si>
-  <si>
-    <t>◾ separates complex object construction from representation</t>
-  </si>
-  <si>
-    <t>[3.] Factory Method</t>
-  </si>
-  <si>
-    <t>◾ defines an interface for creating objects</t>
-  </si>
-  <si>
-    <t>◾ allows subclasses to choose the concrete class to instantiate</t>
-  </si>
-  <si>
-    <t>[4.] Prototype</t>
-  </si>
-  <si>
-    <t>◾ creates new objects by copying a prototypical instance</t>
-  </si>
-  <si>
-    <t>[5.] Singleton</t>
-  </si>
-  <si>
-    <t>◾ ensures a class has only one instance</t>
-  </si>
-  <si>
-    <t>📌 𝐒𝐭𝐫𝐮𝐜𝐭𝐮𝐫𝐚𝐥 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬</t>
-  </si>
-  <si>
-    <t>[6.] Adapter</t>
-  </si>
-  <si>
-    <t>◾ converts one interface to another, allowing incompatible classes to work together</t>
-  </si>
-  <si>
-    <t>[7.] Bridge</t>
-  </si>
-  <si>
-    <t>◾ decouples abstraction and implementation, enabling independent variation</t>
-  </si>
-  <si>
-    <t>[8.] Composite</t>
-  </si>
-  <si>
-    <t>◾ treats individual objects &amp; their compositions uniformly, representing part-whole hierarchies</t>
-  </si>
-  <si>
-    <t>[9.] Decorator</t>
-  </si>
-  <si>
-    <t>◾ dynamically adds responsibilities to an object without subclassing</t>
-  </si>
-  <si>
-    <t>[10.] Facade</t>
-  </si>
-  <si>
-    <t>◾ provides a simplified interface to a complex subsystem</t>
-  </si>
-  <si>
-    <t>[11.] Flyweight</t>
-  </si>
-  <si>
-    <t>◾ shares objects to reduce memory usage for large numbers of fine-grained objects</t>
-  </si>
-  <si>
-    <t>[12.] Proxy</t>
-  </si>
-  <si>
-    <t>◾ controls access to an object, offering various capabilities like lazy loading or remote access</t>
-  </si>
-  <si>
-    <t>📌 𝐁𝐞𝐡𝐚𝐯𝐢𝐨𝐫𝐚𝐥 𝐏𝐚𝐭𝐭𝐞𝐫𝐧𝐬</t>
-  </si>
-  <si>
-    <t>[13.] Chain of Responsibility</t>
-  </si>
-  <si>
-    <t>◾ decouples request senders and receivers, allowing multiple objects to handle the request</t>
-  </si>
-  <si>
-    <t>[14.] Command</t>
-  </si>
-  <si>
-    <t>◾ encapsulates requests as objects, enabling logging, queuing, and undo/redo operations</t>
-  </si>
-  <si>
-    <t>[15.] Interpreter</t>
-  </si>
-  <si>
-    <t>◾ defines a grammar for a language and an interpreter to execute expressions</t>
-  </si>
-  <si>
-    <t>[16.] Iterator</t>
-  </si>
-  <si>
-    <t>◾ provides sequential access to aggregate elements without exposing the underlying representation</t>
-  </si>
-  <si>
-    <t>[17.] Mediator</t>
-  </si>
-  <si>
-    <t>◾ encapsulates object interaction, promoting loose coupling</t>
-  </si>
-  <si>
-    <t>[18.] Memento</t>
-  </si>
-  <si>
-    <t>◾ captures and restores an object's state without violating encapsulation</t>
-  </si>
-  <si>
-    <t>[19.] Observer</t>
-  </si>
-  <si>
-    <t>◾ notifies dependents automatically when an object's state changes</t>
-  </si>
-  <si>
-    <t>[20.] State</t>
-  </si>
-  <si>
-    <t>◾ alters an object's behavior when its internal state changes</t>
-  </si>
-  <si>
-    <t>[21.] Strategy</t>
-  </si>
-  <si>
-    <t>◾ encapsulates interchangeable algorithms, allowing clients to choose dynamically</t>
-  </si>
-  <si>
-    <t>[22.] Template</t>
-  </si>
-  <si>
-    <t>◾ defines the skeleton of an algorithm, deferring steps to subclasses</t>
-  </si>
-  <si>
-    <t>[23.] Visitor</t>
-  </si>
-  <si>
-    <t>◾ adds new operations to object structures without modifying the element classes</t>
-  </si>
-  <si>
-    <t>While design patterns are conceptual, their proper application is often reflected in consistent structure, naming, and abstraction. Tools like CodeRabbit help catch inconsistencies and code smells during reviews, making it easier to maintain pattern-aligned code as projects scale.</t>
   </si>
 </sst>
 </file>
@@ -1077,13 +1077,6 @@
   <fonts count="26">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1108,6 +1101,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1751,32 +1751,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2350,6 +2350,327 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="R3:R86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetData>
+    <row r="3" spans="18:18">
+      <c r="R3" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="18:18">
+      <c r="R4" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="18:18">
+      <c r="R5" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="18:18">
+      <c r="R6" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="18:18">
+      <c r="R7" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="18:18">
+      <c r="R8" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="18:18">
+      <c r="R9" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="18:18">
+      <c r="R10" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="18:18">
+      <c r="R11" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="18:18">
+      <c r="R13" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="18:18">
+      <c r="R14" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="18:18">
+      <c r="R15" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="18:18">
+      <c r="R17" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="18:18">
+      <c r="R18" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="18:18">
+      <c r="R20" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="18:18">
+      <c r="R21" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="18:18">
+      <c r="R22" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="18:18">
+      <c r="R24" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="18:18">
+      <c r="R25" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="18:18">
+      <c r="R27" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="18:18">
+      <c r="R28" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="18:18">
+      <c r="R30" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="18:18">
+      <c r="R31" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="18:18">
+      <c r="R32" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="18:18">
+      <c r="R34" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="18:18">
+      <c r="R35" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="18:18">
+      <c r="R37" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="18:18">
+      <c r="R38" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="18:18">
+      <c r="R40" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="18:18">
+      <c r="R41" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="18:18">
+      <c r="R43" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="18:18">
+      <c r="R44" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="18:18">
+      <c r="R46" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="18:18">
+      <c r="R47" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="18:18">
+      <c r="R49" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="18:18">
+      <c r="R50" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="18:18">
+      <c r="R52" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="18:18">
+      <c r="R53" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="18:18">
+      <c r="R54" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="18:18">
+      <c r="R56" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="18:18">
+      <c r="R57" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="18:18">
+      <c r="R59" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="18:18">
+      <c r="R60" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="18:18">
+      <c r="R62" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="63" spans="18:18">
+      <c r="R63" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="18:18">
+      <c r="R65" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="18:18">
+      <c r="R66" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="68" spans="18:18">
+      <c r="R68" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="18:18">
+      <c r="R69" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="18:18">
+      <c r="R71" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="18:18">
+      <c r="R72" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="18:18">
+      <c r="R74" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="75" spans="18:18">
+      <c r="R75" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="18:18">
+      <c r="R77" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="78" spans="18:18">
+      <c r="R78" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="18:18">
+      <c r="R80" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" spans="18:18">
+      <c r="R81" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="18:18">
+      <c r="R83" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" spans="18:18">
+      <c r="R84" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="86" spans="18:18">
+      <c r="R86" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="R86" r:id="rId2" display="While design patterns are conceptual, their proper application is often reflected in consistent structure, naming, and abstraction. Tools like CodeRabbit help catch inconsistencies and code smells during reviews, making it easier to maintain pattern-aligned code as projects scale." tooltip="https://www.linkedin.com/company/coderabbitai/"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B2:J9"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
@@ -2367,160 +2688,160 @@
   </cols>
   <sheetData>
     <row r="2" ht="19.2" spans="2:8">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" ht="36" spans="2:8">
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" ht="106" spans="2:8">
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>14</v>
+      <c r="B4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="5" ht="106" spans="2:10">
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="6"/>
+      <c r="B5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" ht="88" spans="2:10">
-      <c r="B6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="6"/>
+      <c r="B6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" ht="106" spans="2:10">
-      <c r="B7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" ht="88" spans="2:10">
-      <c r="B8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J8" s="6"/>
+      <c r="B8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" ht="17.6" spans="10:10">
-      <c r="J9" s="6"/>
+      <c r="J9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2531,7 +2852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="B2:M13"/>
@@ -2551,176 +2872,176 @@
   </cols>
   <sheetData>
     <row r="2" ht="19.2" spans="2:8">
-      <c r="B2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="B2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" ht="36" spans="2:8">
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" ht="106" spans="2:8">
-      <c r="B4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>50</v>
+      <c r="B4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="5" ht="71" spans="2:10">
-      <c r="B5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="6"/>
+      <c r="B5" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" ht="71" spans="2:10">
-      <c r="B6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" ht="88" spans="2:10">
-      <c r="B7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J7" s="6"/>
+      <c r="B7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" ht="88" spans="2:13">
-      <c r="B8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
+      <c r="B8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" ht="17.6" spans="10:11">
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
     </row>
     <row r="10" ht="17.6" spans="11:11">
-      <c r="K10" s="6"/>
+      <c r="K10" s="5"/>
     </row>
     <row r="11" ht="17.6" spans="11:11">
-      <c r="K11" s="6"/>
+      <c r="K11" s="5"/>
     </row>
     <row r="12" ht="17.6" spans="11:11">
-      <c r="K12" s="6"/>
+      <c r="K12" s="5"/>
     </row>
     <row r="13" ht="17.6" spans="11:11">
-      <c r="K13" s="6"/>
+      <c r="K13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2731,7 +3052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="B2:L13"/>
@@ -2751,283 +3072,283 @@
   </cols>
   <sheetData>
     <row r="2" ht="19.2" spans="2:8">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" ht="36" spans="2:8">
-      <c r="B3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>7</v>
+      <c r="B3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" ht="88" spans="2:12">
-      <c r="B4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="B4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" ht="88" spans="2:12">
-      <c r="B5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="B5" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" ht="88" spans="2:12">
-      <c r="B6" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="B6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" ht="106" spans="2:12">
-      <c r="B7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" ht="88" spans="2:12">
-      <c r="B8" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="B8" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" ht="88" spans="2:12">
-      <c r="B9" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="L9" s="6"/>
+      <c r="B9" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" ht="88" spans="2:12">
-      <c r="B10" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="L10" s="6"/>
+      <c r="B10" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" ht="88" spans="2:12">
-      <c r="B11" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="L11" s="6"/>
+      <c r="B11" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" ht="88" spans="2:12">
-      <c r="B12" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="L12" s="6"/>
+      <c r="B12" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="L12" s="5"/>
     </row>
     <row r="13" ht="88" spans="2:12">
-      <c r="B13" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="L13" s="6"/>
+      <c r="B13" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="L13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3036,325 +3357,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="R3:R86"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:R86"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
-  <sheetData>
-    <row r="3" spans="18:18">
-      <c r="R3" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="18:18">
-      <c r="R4" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="18:18">
-      <c r="R5" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="18:18">
-      <c r="R6" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="18:18">
-      <c r="R7" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="18:18">
-      <c r="R8" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="18:18">
-      <c r="R9" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="10" spans="18:18">
-      <c r="R10" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="18:18">
-      <c r="R11" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="18:18">
-      <c r="R13" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="14" spans="18:18">
-      <c r="R14" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="15" spans="18:18">
-      <c r="R15" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="18:18">
-      <c r="R17" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="18:18">
-      <c r="R18" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="18:18">
-      <c r="R20" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="18:18">
-      <c r="R21" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="18:18">
-      <c r="R22" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="18:18">
-      <c r="R24" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="25" spans="18:18">
-      <c r="R25" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="18:18">
-      <c r="R27" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="28" spans="18:18">
-      <c r="R28" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="30" spans="18:18">
-      <c r="R30" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="18:18">
-      <c r="R31" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="32" spans="18:18">
-      <c r="R32" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="18:18">
-      <c r="R34" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="35" spans="18:18">
-      <c r="R35" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="37" spans="18:18">
-      <c r="R37" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="18:18">
-      <c r="R38" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="40" spans="18:18">
-      <c r="R40" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="18:18">
-      <c r="R41" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="43" spans="18:18">
-      <c r="R43" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="44" spans="18:18">
-      <c r="R44" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="46" spans="18:18">
-      <c r="R46" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="47" spans="18:18">
-      <c r="R47" s="1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="49" spans="18:18">
-      <c r="R49" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="50" spans="18:18">
-      <c r="R50" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="52" spans="18:18">
-      <c r="R52" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="53" spans="18:18">
-      <c r="R53" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="54" spans="18:18">
-      <c r="R54" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="56" spans="18:18">
-      <c r="R56" s="1" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="57" spans="18:18">
-      <c r="R57" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="59" spans="18:18">
-      <c r="R59" s="1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="60" spans="18:18">
-      <c r="R60" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="62" spans="18:18">
-      <c r="R62" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="18:18">
-      <c r="R63" s="1" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="65" spans="18:18">
-      <c r="R65" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="66" spans="18:18">
-      <c r="R66" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="68" spans="18:18">
-      <c r="R68" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="69" spans="18:18">
-      <c r="R69" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="71" spans="18:18">
-      <c r="R71" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="72" spans="18:18">
-      <c r="R72" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="74" spans="18:18">
-      <c r="R74" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="75" spans="18:18">
-      <c r="R75" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="77" spans="18:18">
-      <c r="R77" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="78" spans="18:18">
-      <c r="R78" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="80" spans="18:18">
-      <c r="R80" s="1" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="81" spans="18:18">
-      <c r="R81" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="83" spans="18:18">
-      <c r="R83" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="84" spans="18:18">
-      <c r="R84" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="86" spans="18:18">
-      <c r="R86" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="R86" r:id="rId2" display="While design patterns are conceptual, their proper application is often reflected in consistent structure, naming, and abstraction. Tools like CodeRabbit help catch inconsistencies and code smells during reviews, making it easier to maintain pattern-aligned code as projects scale." tooltip="https://www.linkedin.com/company/coderabbitai/"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>